<commit_message>
Uitgangssituatie (stap1, nu via radio-button 2023) en Holon-warmtenet (stap 2, via radio button 2027)
</commit_message>
<xml_diff>
--- a/Data/House_thermal_parameters.xlsx
+++ b/Data/House_thermal_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gilli\Documents\Project HOLON\Git_Local_Clone\HOLON\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FBF427C-40E7-499A-BE5D-15E898D77FD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74797905-259B-4A39-85A5-CBF4D4BFC5B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3855" yWindow="4695" windowWidth="38700" windowHeight="15435" activeTab="1" xr2:uid="{208BE1E8-6DE5-4A2F-ABE4-805A1B8EE376}"/>
+    <workbookView xWindow="8475" yWindow="1200" windowWidth="38700" windowHeight="19395" activeTab="1" xr2:uid="{208BE1E8-6DE5-4A2F-ABE4-805A1B8EE376}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="50">
   <si>
     <t>Value</t>
   </si>
@@ -183,6 +183,9 @@
   </si>
   <si>
     <t>Ventilatiedebiet</t>
+  </si>
+  <si>
+    <t>MJ</t>
   </si>
 </sst>
 </file>
@@ -627,10 +630,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45CCD2A0-BA9C-4455-9EB8-D7257747F670}">
-  <dimension ref="B1:F25"/>
+  <dimension ref="B1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,12 +641,12 @@
     <col min="3" max="3" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>8</v>
       </c>
@@ -654,7 +657,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>4</v>
       </c>
@@ -665,7 +668,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>21</v>
       </c>
@@ -676,8 +679,15 @@
       <c r="E4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <f>D4*3600000/1000000000</f>
+        <v>3.5171999999999999</v>
+      </c>
+      <c r="G4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>27</v>
       </c>
@@ -688,7 +698,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>23</v>
       </c>
@@ -700,12 +710,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>5</v>
       </c>
@@ -716,7 +726,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>6</v>
       </c>
@@ -727,7 +737,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>25</v>
       </c>
@@ -739,7 +749,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>48</v>
       </c>
@@ -751,7 +761,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>31</v>
       </c>
@@ -763,7 +773,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>20</v>
       </c>
@@ -775,7 +785,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>34</v>
       </c>

</xml_diff>